<commit_message>
Carpetas Faltantes. Actualizacion de scripts
</commit_message>
<xml_diff>
--- a/Documentacion Progreso.xlsx
+++ b/Documentacion Progreso.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="80">
   <si>
     <t>Nombre Entidad</t>
   </si>
@@ -210,14 +207,65 @@
     <t>Mobile_Handset_Sale</t>
   </si>
   <si>
-    <t>0-100</t>
+    <t>D_Mobile_Billing_Cycle</t>
+  </si>
+  <si>
+    <t>Mobile_Movement</t>
+  </si>
+  <si>
+    <t>Control de Gestión</t>
+  </si>
+  <si>
+    <t>MOBILE_REVENUE</t>
+  </si>
+  <si>
+    <t>Mobile_Line</t>
+  </si>
+  <si>
+    <t>IMEI_HIST</t>
+  </si>
+  <si>
+    <t>D_AgeSegment</t>
+  </si>
+  <si>
+    <t>D_Geographical_Area</t>
+  </si>
+  <si>
+    <t>D_Geographical_Area_Rel</t>
+  </si>
+  <si>
+    <t>D_Geographical_Area_Type</t>
+  </si>
+  <si>
+    <t>D_Line_Status</t>
+  </si>
+  <si>
+    <t>D_Mobile_Line_Type</t>
+  </si>
+  <si>
+    <t>D_Mobile_PrePostpaid</t>
+  </si>
+  <si>
+    <t>D_Movement_Type</t>
+  </si>
+  <si>
+    <t>D_Port_Operator</t>
+  </si>
+  <si>
+    <t>D_Segment</t>
+  </si>
+  <si>
+    <t>IMEI_TAC</t>
+  </si>
+  <si>
+    <t>0-5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +276,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -254,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -270,6 +341,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,10 +637,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,827 +653,905 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>25</v>
-      </c>
+      <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="7">
         <v>0</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>26</v>
-      </c>
+    <row r="4" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>27</v>
-      </c>
+      <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4">
+        <v>63</v>
+      </c>
+      <c r="C5" s="7">
         <v>0</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>28</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4">
+        <v>64</v>
+      </c>
+      <c r="C6" s="7">
         <v>0</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>29</v>
-      </c>
+      <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="4">
+        <v>64</v>
+      </c>
+      <c r="C7" s="7">
         <v>0</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>30</v>
-      </c>
+      <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="C8" s="7">
+        <v>2</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>31</v>
-      </c>
+      <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>32</v>
-      </c>
+      <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>33</v>
-      </c>
+      <c r="A11" s="3"/>
       <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="4">
+        <v>66</v>
+      </c>
+      <c r="C11" s="7">
         <v>0</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>34</v>
-      </c>
+      <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="4">
+        <v>66</v>
+      </c>
+      <c r="C12" s="7">
         <v>0</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>35</v>
-      </c>
+      <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>36</v>
-      </c>
+      <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4">
+        <v>68</v>
+      </c>
+      <c r="C14" s="7">
         <v>0</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>37</v>
-      </c>
+      <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0</v>
+        <v>69</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>38</v>
-      </c>
+      <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="C16" s="7">
+        <v>2</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>39</v>
-      </c>
+      <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0</v>
+        <v>71</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>40</v>
-      </c>
+      <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="4">
+        <v>72</v>
+      </c>
+      <c r="C18" s="7">
         <v>0</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>41</v>
-      </c>
+      <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="4">
+        <v>73</v>
+      </c>
+      <c r="C19" s="7">
         <v>0</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>42</v>
-      </c>
+      <c r="A20" s="3"/>
       <c r="B20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="4">
+        <v>74</v>
+      </c>
+      <c r="C20" s="7">
         <v>0</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>43</v>
-      </c>
+      <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0</v>
+        <v>75</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>44</v>
-      </c>
+      <c r="A22" s="3"/>
       <c r="B22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="C22" s="7">
+        <v>2</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>45</v>
-      </c>
+      <c r="A23" s="3"/>
       <c r="B23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="4">
+        <v>77</v>
+      </c>
+      <c r="C23" s="7">
         <v>0</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>46</v>
-      </c>
+      <c r="A24" s="3"/>
       <c r="B24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0</v>
+        <v>78</v>
+      </c>
+      <c r="C24" s="7">
+        <v>2</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>47</v>
-      </c>
+      <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="4">
+        <v>78</v>
+      </c>
+      <c r="C25" s="7">
         <v>0</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>48</v>
-      </c>
+      <c r="A26" s="3"/>
       <c r="B26" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="4">
+        <v>61</v>
+      </c>
+      <c r="C26" s="7">
         <v>0</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>49</v>
-      </c>
+      <c r="A27" s="3"/>
       <c r="B27" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="C27" s="7">
+        <v>2</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>50</v>
-      </c>
+      <c r="A28" s="3"/>
       <c r="B28" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="4">
+        <v>4</v>
+      </c>
+      <c r="C28" s="7">
         <v>0</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>51</v>
-      </c>
+      <c r="A29" s="3"/>
       <c r="B29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="4">
+        <v>5</v>
+      </c>
+      <c r="C29" s="7">
         <v>0</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>52</v>
-      </c>
+      <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="4">
+        <v>6</v>
+      </c>
+      <c r="C30" s="7">
         <v>0</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>53</v>
-      </c>
+      <c r="A31" s="3"/>
       <c r="B31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="4">
+        <v>7</v>
+      </c>
+      <c r="C31" s="7">
         <v>0</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>54</v>
-      </c>
+      <c r="A32" s="3"/>
       <c r="B32" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="4">
+        <v>8</v>
+      </c>
+      <c r="C32" s="7">
         <v>0</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>55</v>
-      </c>
+      <c r="A33" s="3"/>
       <c r="B33" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="4">
+        <v>9</v>
+      </c>
+      <c r="C33" s="7">
         <v>0</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>56</v>
-      </c>
+      <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="4">
+        <v>10</v>
+      </c>
+      <c r="C34" s="7">
         <v>0</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>57</v>
-      </c>
+      <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="4">
+        <v>11</v>
+      </c>
+      <c r="C35" s="7">
         <v>0</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>58</v>
-      </c>
+      <c r="A36" s="3"/>
       <c r="B36" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="4">
+        <v>12</v>
+      </c>
+      <c r="C36" s="7">
         <v>0</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>59</v>
-      </c>
+      <c r="A37" s="3"/>
       <c r="B37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="4">
+        <v>13</v>
+      </c>
+      <c r="C37" s="7">
         <v>0</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>60</v>
-      </c>
+      <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="4">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="C38" s="7">
+        <v>3</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>61</v>
-      </c>
+      <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="4">
+        <v>15</v>
+      </c>
+      <c r="C39" s="7">
         <v>0</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>62</v>
-      </c>
+      <c r="A40" s="3"/>
       <c r="B40" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="4">
+        <v>16</v>
+      </c>
+      <c r="C40" s="7">
         <v>0</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>63</v>
-      </c>
+      <c r="A41" s="3"/>
       <c r="B41" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="4">
+        <v>17</v>
+      </c>
+      <c r="C41" s="7">
         <v>0</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>64</v>
-      </c>
+      <c r="A42" s="3"/>
       <c r="B42" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="4">
+        <v>18</v>
+      </c>
+      <c r="C42" s="7">
         <v>0</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <v>65</v>
-      </c>
+      <c r="A43" s="3"/>
       <c r="B43" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="4">
+        <v>19</v>
+      </c>
+      <c r="C43" s="7">
         <v>0</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
     </row>
     <row r="44" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>66</v>
-      </c>
+      <c r="A44" s="3"/>
       <c r="B44" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" s="4">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="C44" s="7">
+        <v>2</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
     </row>
     <row r="45" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>67</v>
-      </c>
+      <c r="A45" s="3"/>
       <c r="B45" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" s="4">
+        <v>21</v>
+      </c>
+      <c r="C45" s="7">
         <v>0</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
     </row>
     <row r="46" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>68</v>
-      </c>
+      <c r="A46" s="3"/>
       <c r="B46" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" s="4">
+        <v>22</v>
+      </c>
+      <c r="C46" s="7">
         <v>0</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
     </row>
     <row r="47" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>69</v>
-      </c>
+      <c r="A47" s="3"/>
       <c r="B47" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" s="4">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="C47" s="7">
+        <v>3</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
     </row>
     <row r="48" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>70</v>
-      </c>
+      <c r="A48" s="3"/>
       <c r="B48" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="4">
+        <v>24</v>
+      </c>
+      <c r="C48" s="7">
         <v>0</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
-        <v>71</v>
-      </c>
+      <c r="A49" s="3"/>
       <c r="B49" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49" s="4">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="C49" s="7">
+        <v>2</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
     </row>
     <row r="50" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
-        <v>72</v>
-      </c>
+      <c r="A50" s="3"/>
       <c r="B50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" s="4">
+        <v>26</v>
+      </c>
+      <c r="C50" s="7">
         <v>0</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
     </row>
     <row r="51" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
-        <v>73</v>
-      </c>
+      <c r="A51" s="3"/>
       <c r="B51" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" s="4">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="C51" s="7">
+        <v>3</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
     </row>
     <row r="52" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
-        <v>74</v>
-      </c>
+      <c r="A52" s="3"/>
       <c r="B52" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" s="4">
+        <v>28</v>
+      </c>
+      <c r="C52" s="7">
         <v>0</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
     </row>
     <row r="53" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
-        <v>75</v>
-      </c>
+      <c r="A53" s="3"/>
       <c r="B53" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C53" s="4">
+        <v>29</v>
+      </c>
+      <c r="C53" s="7">
         <v>0</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
     </row>
     <row r="54" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
-        <v>76</v>
-      </c>
+      <c r="A54" s="3"/>
       <c r="B54" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C54" s="4">
+        <v>30</v>
+      </c>
+      <c r="C54" s="7">
         <v>0</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
     </row>
     <row r="55" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
-        <v>77</v>
-      </c>
+      <c r="A55" s="3"/>
       <c r="B55" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C55" s="4">
+        <v>31</v>
+      </c>
+      <c r="C55" s="7">
         <v>0</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
     </row>
     <row r="56" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3">
-        <v>78</v>
-      </c>
+      <c r="A56" s="3"/>
       <c r="B56" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C56" s="4">
+        <v>32</v>
+      </c>
+      <c r="C56" s="7">
         <v>0</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
     </row>
     <row r="57" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3">
-        <v>79</v>
-      </c>
+      <c r="A57" s="3"/>
       <c r="B57" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C57" s="4">
+        <v>33</v>
+      </c>
+      <c r="C57" s="7">
         <v>0</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3">
-        <v>80</v>
-      </c>
+      <c r="A58" s="3"/>
       <c r="B58" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C58" s="4">
+        <v>34</v>
+      </c>
+      <c r="C58" s="7">
         <v>0</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
     </row>
     <row r="59" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3">
-        <v>81</v>
-      </c>
+      <c r="A59" s="3"/>
       <c r="B59" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="4">
+        <v>35</v>
+      </c>
+      <c r="C59" s="7">
         <v>0</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
     </row>
     <row r="60" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3">
-        <v>82</v>
-      </c>
+      <c r="A60" s="3"/>
       <c r="B60" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C60" s="4">
+        <v>36</v>
+      </c>
+      <c r="C60" s="7">
         <v>0</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
     </row>
     <row r="61" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4">
-        <v>4</v>
+      <c r="A61" s="3"/>
+      <c r="B61" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="7">
+        <v>0</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
     </row>
+    <row r="62" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="B62" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" t="s">
+        <v>39</v>
+      </c>
+      <c r="C63" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" t="s">
+        <v>43</v>
+      </c>
+      <c r="C67" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" t="s">
+        <v>47</v>
+      </c>
+      <c r="C71" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+      <c r="B72" t="s">
+        <v>48</v>
+      </c>
+      <c r="C72" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+      <c r="B73" t="s">
+        <v>49</v>
+      </c>
+      <c r="C73" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="B74" t="s">
+        <v>50</v>
+      </c>
+      <c r="C74" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" t="s">
+        <v>51</v>
+      </c>
+      <c r="C75" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" t="s">
+        <v>52</v>
+      </c>
+      <c r="C76" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+      <c r="B77" t="s">
+        <v>53</v>
+      </c>
+      <c r="C77" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+      <c r="B78" t="s">
+        <v>54</v>
+      </c>
+      <c r="C78" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+      <c r="B79" t="s">
+        <v>55</v>
+      </c>
+      <c r="C79" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+      <c r="B80" t="s">
+        <v>56</v>
+      </c>
+      <c r="C80" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+      <c r="B81" t="s">
+        <v>57</v>
+      </c>
+      <c r="C81" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+      <c r="B82" t="s">
+        <v>58</v>
+      </c>
+      <c r="C82" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+      <c r="B83" t="s">
+        <v>60</v>
+      </c>
+      <c r="C83" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+      <c r="C84" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:C61">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
+  <conditionalFormatting sqref="C3:C84">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
         <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{ED501BD9-504C-471F-927D-1C97F93DE87C}</x14:id>
-        </ext>
-      </extLst>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="50" fitToWidth="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{ED501BD9-504C-471F-927D-1C97F93DE87C}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>C3:C61</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>